<commit_message>
add regression for data ex china, fix Korea in WEO
</commit_message>
<xml_diff>
--- a/data_plot_avgIndex_gdp.xlsx
+++ b/data_plot_avgIndex_gdp.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>country</t>
   </si>
@@ -122,6 +122,9 @@
     <t>33</t>
   </si>
   <si>
+    <t>34</t>
+  </si>
+  <si>
     <t>Australia</t>
   </si>
   <si>
@@ -201,6 +204,9 @@
   </si>
   <si>
     <t>Slovenia</t>
+  </si>
+  <si>
+    <t>South Korea</t>
   </si>
   <si>
     <t>Spain</t>
@@ -286,7 +292,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" t="n">
         <v>42.06967032967033</v>
@@ -300,7 +306,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" t="n">
         <v>40.63983516483516</v>
@@ -314,7 +320,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4" t="n">
         <v>46.183626373626375</v>
@@ -328,7 +334,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" t="n">
         <v>47.29637362637363</v>
@@ -342,7 +348,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" t="n">
         <v>43.01587912087912</v>
@@ -356,7 +362,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" t="n">
         <v>43.567252747252745</v>
@@ -370,7 +376,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" t="n">
         <v>65.38027472527472</v>
@@ -384,7 +390,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" t="n">
         <v>52.996813186813185</v>
@@ -398,7 +404,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C10" t="n">
         <v>40.068131868131864</v>
@@ -412,7 +418,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11" t="n">
         <v>42.30175824175824</v>
@@ -426,7 +432,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" t="n">
         <v>33.996593406593405</v>
@@ -440,7 +446,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C13" t="n">
         <v>53.41505494505494</v>
@@ -454,7 +460,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C14" t="n">
         <v>43.82087912087912</v>
@@ -468,7 +474,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C15" t="n">
         <v>43.5389010989011</v>
@@ -482,7 +488,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C16" t="n">
         <v>41.71120879120879</v>
@@ -496,7 +502,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C17" t="n">
         <v>54.121813186813185</v>
@@ -510,7 +516,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C18" t="n">
         <v>47.378186813186815</v>
@@ -524,7 +530,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C19" t="n">
         <v>48.57565934065934</v>
@@ -538,7 +544,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C20" t="n">
         <v>53.0671978021978</v>
@@ -552,7 +558,7 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C21" t="n">
         <v>54.940714285714286</v>
@@ -566,7 +572,7 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C22" t="n">
         <v>29.81692307692308</v>
@@ -580,7 +586,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C23" t="n">
         <v>42.832802197802195</v>
@@ -594,7 +600,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C24" t="n">
         <v>42.99961538461538</v>
@@ -608,7 +614,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C25" t="n">
         <v>44.52598901098901</v>
@@ -622,7 +628,7 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C26" t="n">
         <v>48.294120879120875</v>
@@ -636,7 +642,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C27" t="n">
         <v>49.50741758241758</v>
@@ -650,7 +656,7 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C28" t="n">
         <v>37.53181318681319</v>
@@ -664,13 +670,13 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C29" t="n">
-        <v>46.89736263736264</v>
+        <v>44.2589010989011</v>
       </c>
       <c r="D29" t="n">
-        <v>-22.738000000000014</v>
+        <v>-4.395130442387327</v>
       </c>
     </row>
     <row r="30">
@@ -678,13 +684,13 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C30" t="n">
-        <v>25.428956043956042</v>
+        <v>46.89736263736264</v>
       </c>
       <c r="D30" t="n">
-        <v>-8.116599999999991</v>
+        <v>-22.738000000000014</v>
       </c>
     </row>
     <row r="31">
@@ -692,13 +698,13 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C31" t="n">
-        <v>40.135274725274726</v>
+        <v>25.428956043956042</v>
       </c>
       <c r="D31" t="n">
-        <v>-10.478372200337631</v>
+        <v>-8.116599999999991</v>
       </c>
     </row>
     <row r="32">
@@ -706,13 +712,13 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C32" t="n">
-        <v>46.23115384615385</v>
+        <v>40.135274725274726</v>
       </c>
       <c r="D32" t="n">
-        <v>-11.13251181519172</v>
+        <v>-10.478372200337631</v>
       </c>
     </row>
     <row r="33">
@@ -720,13 +726,13 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C33" t="n">
-        <v>45.70757142857143</v>
+        <v>46.23115384615385</v>
       </c>
       <c r="D33" t="n">
-        <v>-22.116289412320953</v>
+        <v>-11.13251181519172</v>
       </c>
     </row>
     <row r="34">
@@ -734,12 +740,26 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C34" t="n">
-        <v>44.5439114658926</v>
+        <v>45.70757142857143</v>
       </c>
       <c r="D34" t="n">
+        <v>-22.116289412320953</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" t="n">
+        <v>44.614688990255026</v>
+      </c>
+      <c r="D35" t="n">
         <v>-10.24086007423928</v>
       </c>
     </row>

</xml_diff>